<commit_message>
Google Social SSO login support
</commit_message>
<xml_diff>
--- a/example-devices-inventory.xlsx
+++ b/example-devices-inventory.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/srho/electron-test/jccm-project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3BC263E-1428-5349-A6CE-58332729D9F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{445F0BD7-41AE-7240-8C56-F8669648DAE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -46,9 +46,6 @@
     <t>Site-01</t>
   </si>
   <si>
-    <t>10.6.3.56</t>
-  </si>
-  <si>
     <t>poc</t>
   </si>
   <si>
@@ -64,10 +61,13 @@
     <t>Site-04</t>
   </si>
   <si>
-    <t>10.6.3.55</t>
+    <t>192.168.1.56</t>
   </si>
   <si>
-    <t>10.6.3.54</t>
+    <t>192.168.1.55</t>
+  </si>
+  <si>
+    <t>192.168.1.54</t>
   </si>
 </sst>
 </file>
@@ -446,7 +446,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F97"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
       <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
@@ -454,8 +454,8 @@
   <cols>
     <col min="1" max="1" width="23.83203125" customWidth="1"/>
     <col min="2" max="2" width="7.83203125" customWidth="1"/>
-    <col min="3" max="3" width="9.83203125" customWidth="1"/>
-    <col min="4" max="4" width="4.83203125" customWidth="1"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="4" max="4" width="6.1640625" customWidth="1"/>
     <col min="5" max="6" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -487,16 +487,16 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D2">
         <v>5901</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -507,16 +507,16 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D3">
         <v>5902</v>
       </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -527,16 +527,16 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D4">
         <v>5903</v>
       </c>
       <c r="E4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -547,16 +547,16 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D5">
         <v>5904</v>
       </c>
       <c r="E5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -567,16 +567,16 @@
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D6">
         <v>5905</v>
       </c>
       <c r="E6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -587,16 +587,16 @@
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D7">
         <v>5906</v>
       </c>
       <c r="E7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -607,16 +607,16 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D8">
         <v>5907</v>
       </c>
       <c r="E8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -627,16 +627,16 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D9">
         <v>5908</v>
       </c>
       <c r="E9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -644,19 +644,19 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D10">
         <v>5909</v>
       </c>
       <c r="E10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -664,19 +664,19 @@
         <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D11">
         <v>5910</v>
       </c>
       <c r="E11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -684,19 +684,19 @@
         <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D12">
         <v>5911</v>
       </c>
       <c r="E12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -704,19 +704,19 @@
         <v>6</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D13">
         <v>5912</v>
       </c>
       <c r="E13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -724,19 +724,19 @@
         <v>6</v>
       </c>
       <c r="B14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C14" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D14">
         <v>5913</v>
       </c>
       <c r="E14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -744,19 +744,19 @@
         <v>6</v>
       </c>
       <c r="B15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C15" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D15">
         <v>5914</v>
       </c>
       <c r="E15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -764,19 +764,19 @@
         <v>6</v>
       </c>
       <c r="B16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C16" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D16">
         <v>5915</v>
       </c>
       <c r="E16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -784,19 +784,19 @@
         <v>6</v>
       </c>
       <c r="B17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C17" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D17">
         <v>5916</v>
       </c>
       <c r="E17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -804,19 +804,19 @@
         <v>6</v>
       </c>
       <c r="B18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C18" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D18">
         <v>5917</v>
       </c>
       <c r="E18" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -824,19 +824,19 @@
         <v>6</v>
       </c>
       <c r="B19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C19" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D19">
         <v>5918</v>
       </c>
       <c r="E19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -844,19 +844,19 @@
         <v>6</v>
       </c>
       <c r="B20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C20" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D20">
         <v>5919</v>
       </c>
       <c r="E20" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -864,19 +864,19 @@
         <v>6</v>
       </c>
       <c r="B21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C21" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D21">
         <v>5920</v>
       </c>
       <c r="E21" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -884,19 +884,19 @@
         <v>6</v>
       </c>
       <c r="B22" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C22" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D22">
         <v>5921</v>
       </c>
       <c r="E22" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -904,19 +904,19 @@
         <v>6</v>
       </c>
       <c r="B23" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C23" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D23">
         <v>5922</v>
       </c>
       <c r="E23" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F23" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -924,19 +924,19 @@
         <v>6</v>
       </c>
       <c r="B24" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C24" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D24">
         <v>5923</v>
       </c>
       <c r="E24" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F24" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -944,19 +944,19 @@
         <v>6</v>
       </c>
       <c r="B25" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C25" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D25">
         <v>5924</v>
       </c>
       <c r="E25" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F25" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
@@ -964,19 +964,19 @@
         <v>6</v>
       </c>
       <c r="B26" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C26" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D26">
         <v>5925</v>
       </c>
       <c r="E26" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F26" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -984,19 +984,19 @@
         <v>6</v>
       </c>
       <c r="B27" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C27" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D27">
         <v>5926</v>
       </c>
       <c r="E27" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F27" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -1004,19 +1004,19 @@
         <v>6</v>
       </c>
       <c r="B28" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C28" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D28">
         <v>5927</v>
       </c>
       <c r="E28" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F28" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -1024,19 +1024,19 @@
         <v>6</v>
       </c>
       <c r="B29" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C29" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D29">
         <v>5928</v>
       </c>
       <c r="E29" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F29" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -1044,19 +1044,19 @@
         <v>6</v>
       </c>
       <c r="B30" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C30" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D30">
         <v>5929</v>
       </c>
       <c r="E30" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F30" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
@@ -1064,19 +1064,19 @@
         <v>6</v>
       </c>
       <c r="B31" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C31" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D31">
         <v>5930</v>
       </c>
       <c r="E31" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F31" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
@@ -1084,19 +1084,19 @@
         <v>6</v>
       </c>
       <c r="B32" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C32" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D32">
         <v>5931</v>
       </c>
       <c r="E32" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F32" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
@@ -1104,19 +1104,19 @@
         <v>6</v>
       </c>
       <c r="B33" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C33" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D33">
         <v>5932</v>
       </c>
       <c r="E33" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F33" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
@@ -1133,10 +1133,10 @@
         <v>5901</v>
       </c>
       <c r="E34" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F34" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
@@ -1153,10 +1153,10 @@
         <v>5902</v>
       </c>
       <c r="E35" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F35" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
@@ -1173,10 +1173,10 @@
         <v>5903</v>
       </c>
       <c r="E36" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F36" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
@@ -1193,10 +1193,10 @@
         <v>5904</v>
       </c>
       <c r="E37" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F37" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
@@ -1213,10 +1213,10 @@
         <v>5905</v>
       </c>
       <c r="E38" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F38" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
@@ -1233,10 +1233,10 @@
         <v>5906</v>
       </c>
       <c r="E39" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F39" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
@@ -1253,10 +1253,10 @@
         <v>5907</v>
       </c>
       <c r="E40" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F40" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
@@ -1273,10 +1273,10 @@
         <v>5908</v>
       </c>
       <c r="E41" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F41" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
@@ -1284,7 +1284,7 @@
         <v>6</v>
       </c>
       <c r="B42" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C42" t="s">
         <v>14</v>
@@ -1293,10 +1293,10 @@
         <v>5909</v>
       </c>
       <c r="E42" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F42" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
@@ -1304,7 +1304,7 @@
         <v>6</v>
       </c>
       <c r="B43" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C43" t="s">
         <v>14</v>
@@ -1313,10 +1313,10 @@
         <v>5910</v>
       </c>
       <c r="E43" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F43" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
@@ -1324,7 +1324,7 @@
         <v>6</v>
       </c>
       <c r="B44" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C44" t="s">
         <v>14</v>
@@ -1333,10 +1333,10 @@
         <v>5911</v>
       </c>
       <c r="E44" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F44" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
@@ -1344,7 +1344,7 @@
         <v>6</v>
       </c>
       <c r="B45" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C45" t="s">
         <v>14</v>
@@ -1353,10 +1353,10 @@
         <v>5912</v>
       </c>
       <c r="E45" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F45" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
@@ -1364,7 +1364,7 @@
         <v>6</v>
       </c>
       <c r="B46" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C46" t="s">
         <v>14</v>
@@ -1373,10 +1373,10 @@
         <v>5913</v>
       </c>
       <c r="E46" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F46" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
@@ -1384,7 +1384,7 @@
         <v>6</v>
       </c>
       <c r="B47" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C47" t="s">
         <v>14</v>
@@ -1393,10 +1393,10 @@
         <v>5914</v>
       </c>
       <c r="E47" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F47" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
@@ -1404,7 +1404,7 @@
         <v>6</v>
       </c>
       <c r="B48" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C48" t="s">
         <v>14</v>
@@ -1413,10 +1413,10 @@
         <v>5915</v>
       </c>
       <c r="E48" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F48" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
@@ -1424,7 +1424,7 @@
         <v>6</v>
       </c>
       <c r="B49" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C49" t="s">
         <v>14</v>
@@ -1433,10 +1433,10 @@
         <v>5916</v>
       </c>
       <c r="E49" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F49" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
@@ -1444,7 +1444,7 @@
         <v>6</v>
       </c>
       <c r="B50" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C50" t="s">
         <v>14</v>
@@ -1453,10 +1453,10 @@
         <v>5917</v>
       </c>
       <c r="E50" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F50" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
@@ -1464,7 +1464,7 @@
         <v>6</v>
       </c>
       <c r="B51" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C51" t="s">
         <v>14</v>
@@ -1473,10 +1473,10 @@
         <v>5918</v>
       </c>
       <c r="E51" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F51" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
@@ -1484,7 +1484,7 @@
         <v>6</v>
       </c>
       <c r="B52" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C52" t="s">
         <v>14</v>
@@ -1493,10 +1493,10 @@
         <v>5919</v>
       </c>
       <c r="E52" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F52" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
@@ -1504,7 +1504,7 @@
         <v>6</v>
       </c>
       <c r="B53" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C53" t="s">
         <v>14</v>
@@ -1513,10 +1513,10 @@
         <v>5920</v>
       </c>
       <c r="E53" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F53" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
@@ -1524,7 +1524,7 @@
         <v>6</v>
       </c>
       <c r="B54" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C54" t="s">
         <v>14</v>
@@ -1533,10 +1533,10 @@
         <v>5921</v>
       </c>
       <c r="E54" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F54" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
@@ -1544,7 +1544,7 @@
         <v>6</v>
       </c>
       <c r="B55" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C55" t="s">
         <v>14</v>
@@ -1553,10 +1553,10 @@
         <v>5922</v>
       </c>
       <c r="E55" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F55" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
@@ -1564,7 +1564,7 @@
         <v>6</v>
       </c>
       <c r="B56" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C56" t="s">
         <v>14</v>
@@ -1573,10 +1573,10 @@
         <v>5923</v>
       </c>
       <c r="E56" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F56" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
@@ -1584,7 +1584,7 @@
         <v>6</v>
       </c>
       <c r="B57" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C57" t="s">
         <v>14</v>
@@ -1593,10 +1593,10 @@
         <v>5924</v>
       </c>
       <c r="E57" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F57" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
@@ -1604,7 +1604,7 @@
         <v>6</v>
       </c>
       <c r="B58" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C58" t="s">
         <v>14</v>
@@ -1613,10 +1613,10 @@
         <v>5925</v>
       </c>
       <c r="E58" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F58" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
@@ -1624,7 +1624,7 @@
         <v>6</v>
       </c>
       <c r="B59" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C59" t="s">
         <v>14</v>
@@ -1633,10 +1633,10 @@
         <v>5926</v>
       </c>
       <c r="E59" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F59" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
@@ -1644,7 +1644,7 @@
         <v>6</v>
       </c>
       <c r="B60" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C60" t="s">
         <v>14</v>
@@ -1653,10 +1653,10 @@
         <v>5927</v>
       </c>
       <c r="E60" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F60" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
@@ -1664,7 +1664,7 @@
         <v>6</v>
       </c>
       <c r="B61" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C61" t="s">
         <v>14</v>
@@ -1673,10 +1673,10 @@
         <v>5928</v>
       </c>
       <c r="E61" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F61" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
@@ -1684,7 +1684,7 @@
         <v>6</v>
       </c>
       <c r="B62" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C62" t="s">
         <v>14</v>
@@ -1693,10 +1693,10 @@
         <v>5929</v>
       </c>
       <c r="E62" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F62" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
@@ -1704,7 +1704,7 @@
         <v>6</v>
       </c>
       <c r="B63" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C63" t="s">
         <v>14</v>
@@ -1713,10 +1713,10 @@
         <v>5930</v>
       </c>
       <c r="E63" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F63" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
@@ -1724,7 +1724,7 @@
         <v>6</v>
       </c>
       <c r="B64" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C64" t="s">
         <v>14</v>
@@ -1733,10 +1733,10 @@
         <v>5931</v>
       </c>
       <c r="E64" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F64" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
@@ -1744,7 +1744,7 @@
         <v>6</v>
       </c>
       <c r="B65" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C65" t="s">
         <v>14</v>
@@ -1753,10 +1753,10 @@
         <v>5932</v>
       </c>
       <c r="E65" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F65" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
@@ -1773,10 +1773,10 @@
         <v>5901</v>
       </c>
       <c r="E66" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F66" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
@@ -1793,10 +1793,10 @@
         <v>5902</v>
       </c>
       <c r="E67" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F67" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
@@ -1813,10 +1813,10 @@
         <v>5903</v>
       </c>
       <c r="E68" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F68" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
@@ -1833,10 +1833,10 @@
         <v>5904</v>
       </c>
       <c r="E69" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F69" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
@@ -1853,10 +1853,10 @@
         <v>5905</v>
       </c>
       <c r="E70" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F70" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
@@ -1873,10 +1873,10 @@
         <v>5906</v>
       </c>
       <c r="E71" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F71" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
@@ -1893,10 +1893,10 @@
         <v>5907</v>
       </c>
       <c r="E72" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F72" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
@@ -1913,10 +1913,10 @@
         <v>5908</v>
       </c>
       <c r="E73" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F73" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
@@ -1924,7 +1924,7 @@
         <v>6</v>
       </c>
       <c r="B74" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C74" t="s">
         <v>15</v>
@@ -1933,10 +1933,10 @@
         <v>5909</v>
       </c>
       <c r="E74" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F74" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
@@ -1944,7 +1944,7 @@
         <v>6</v>
       </c>
       <c r="B75" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C75" t="s">
         <v>15</v>
@@ -1953,10 +1953,10 @@
         <v>5910</v>
       </c>
       <c r="E75" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F75" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
@@ -1964,7 +1964,7 @@
         <v>6</v>
       </c>
       <c r="B76" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C76" t="s">
         <v>15</v>
@@ -1973,10 +1973,10 @@
         <v>5911</v>
       </c>
       <c r="E76" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F76" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
@@ -1984,7 +1984,7 @@
         <v>6</v>
       </c>
       <c r="B77" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C77" t="s">
         <v>15</v>
@@ -1993,10 +1993,10 @@
         <v>5912</v>
       </c>
       <c r="E77" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F77" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
@@ -2004,7 +2004,7 @@
         <v>6</v>
       </c>
       <c r="B78" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C78" t="s">
         <v>15</v>
@@ -2013,10 +2013,10 @@
         <v>5913</v>
       </c>
       <c r="E78" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F78" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
@@ -2024,7 +2024,7 @@
         <v>6</v>
       </c>
       <c r="B79" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C79" t="s">
         <v>15</v>
@@ -2033,10 +2033,10 @@
         <v>5914</v>
       </c>
       <c r="E79" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F79" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
@@ -2044,7 +2044,7 @@
         <v>6</v>
       </c>
       <c r="B80" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C80" t="s">
         <v>15</v>
@@ -2053,10 +2053,10 @@
         <v>5915</v>
       </c>
       <c r="E80" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F80" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
@@ -2064,7 +2064,7 @@
         <v>6</v>
       </c>
       <c r="B81" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C81" t="s">
         <v>15</v>
@@ -2073,10 +2073,10 @@
         <v>5916</v>
       </c>
       <c r="E81" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F81" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.2">
@@ -2084,7 +2084,7 @@
         <v>6</v>
       </c>
       <c r="B82" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C82" t="s">
         <v>15</v>
@@ -2093,10 +2093,10 @@
         <v>5917</v>
       </c>
       <c r="E82" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F82" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.2">
@@ -2104,7 +2104,7 @@
         <v>6</v>
       </c>
       <c r="B83" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C83" t="s">
         <v>15</v>
@@ -2113,10 +2113,10 @@
         <v>5918</v>
       </c>
       <c r="E83" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F83" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.2">
@@ -2124,7 +2124,7 @@
         <v>6</v>
       </c>
       <c r="B84" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C84" t="s">
         <v>15</v>
@@ -2133,10 +2133,10 @@
         <v>5919</v>
       </c>
       <c r="E84" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F84" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.2">
@@ -2144,7 +2144,7 @@
         <v>6</v>
       </c>
       <c r="B85" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C85" t="s">
         <v>15</v>
@@ -2153,10 +2153,10 @@
         <v>5920</v>
       </c>
       <c r="E85" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F85" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.2">
@@ -2164,7 +2164,7 @@
         <v>6</v>
       </c>
       <c r="B86" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C86" t="s">
         <v>15</v>
@@ -2173,10 +2173,10 @@
         <v>5921</v>
       </c>
       <c r="E86" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F86" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.2">
@@ -2184,7 +2184,7 @@
         <v>6</v>
       </c>
       <c r="B87" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C87" t="s">
         <v>15</v>
@@ -2193,10 +2193,10 @@
         <v>5922</v>
       </c>
       <c r="E87" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F87" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.2">
@@ -2204,7 +2204,7 @@
         <v>6</v>
       </c>
       <c r="B88" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C88" t="s">
         <v>15</v>
@@ -2213,10 +2213,10 @@
         <v>5923</v>
       </c>
       <c r="E88" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F88" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.2">
@@ -2224,7 +2224,7 @@
         <v>6</v>
       </c>
       <c r="B89" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C89" t="s">
         <v>15</v>
@@ -2233,10 +2233,10 @@
         <v>5924</v>
       </c>
       <c r="E89" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F89" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.2">
@@ -2244,7 +2244,7 @@
         <v>6</v>
       </c>
       <c r="B90" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C90" t="s">
         <v>15</v>
@@ -2253,10 +2253,10 @@
         <v>5925</v>
       </c>
       <c r="E90" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F90" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.2">
@@ -2264,7 +2264,7 @@
         <v>6</v>
       </c>
       <c r="B91" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C91" t="s">
         <v>15</v>
@@ -2273,10 +2273,10 @@
         <v>5926</v>
       </c>
       <c r="E91" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F91" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.2">
@@ -2284,7 +2284,7 @@
         <v>6</v>
       </c>
       <c r="B92" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C92" t="s">
         <v>15</v>
@@ -2293,10 +2293,10 @@
         <v>5927</v>
       </c>
       <c r="E92" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F92" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.2">
@@ -2304,7 +2304,7 @@
         <v>6</v>
       </c>
       <c r="B93" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C93" t="s">
         <v>15</v>
@@ -2313,10 +2313,10 @@
         <v>5928</v>
       </c>
       <c r="E93" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F93" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.2">
@@ -2324,7 +2324,7 @@
         <v>6</v>
       </c>
       <c r="B94" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C94" t="s">
         <v>15</v>
@@ -2333,10 +2333,10 @@
         <v>5929</v>
       </c>
       <c r="E94" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F94" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.2">
@@ -2344,7 +2344,7 @@
         <v>6</v>
       </c>
       <c r="B95" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C95" t="s">
         <v>15</v>
@@ -2353,10 +2353,10 @@
         <v>5930</v>
       </c>
       <c r="E95" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F95" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.2">
@@ -2364,7 +2364,7 @@
         <v>6</v>
       </c>
       <c r="B96" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C96" t="s">
         <v>15</v>
@@ -2373,10 +2373,10 @@
         <v>5931</v>
       </c>
       <c r="E96" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F96" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.2">
@@ -2384,7 +2384,7 @@
         <v>6</v>
       </c>
       <c r="B97" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C97" t="s">
         <v>15</v>
@@ -2393,10 +2393,10 @@
         <v>5932</v>
       </c>
       <c r="E97" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F97" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -2405,7 +2405,7 @@
     <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;7&amp;K000000 Juniper Business Use Only</oddFooter>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="A1:F97" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:F1 A97:B97 A2:B2 D2:F2 A3:B3 D3:F3 A4:B4 D4:F4 A5:B5 D5:F5 A6:B6 D6:F6 A7:B7 D7:F7 A8:B8 D8:F8 A9:B9 D9:F9 A10:B10 D10:F10 A11:B11 D11:F11 A12:B12 D12:F12 A13:B13 D13:F13 A14:B14 D14:F14 A15:B15 D15:F15 A16:B16 D16:F16 A17:B17 D17:F17 A18:B18 D18:F18 A19:B19 D19:F19 A20:B20 D20:F20 A21:B21 D21:F21 A22:B22 D22:F22 A23:B23 D23:F23 A24:B24 D24:F24 A25:B25 D25:F25 A26:B26 D26:F26 A27:B27 D27:F27 A28:B28 D28:F28 A29:B29 D29:F29 A30:B30 D30:F30 A31:B31 D31:F31 A32:B32 D32:F32 A33:B33 D33:F33 A34:B34 D34:F34 A35:B35 D35:F35 A36:B36 D36:F36 A37:B37 D37:F37 A38:B38 D38:F38 A39:B39 D39:F39 A40:B40 D40:F40 A41:B41 D41:F41 A42:B42 D42:F42 A43:B43 D43:F43 A44:B44 D44:F44 A45:B45 D45:F45 A46:B46 D46:F46 A47:B47 D47:F47 A48:B48 D48:F48 A49:B49 D49:F49 A50:B50 D50:F50 A51:B51 D51:F51 A52:B52 D52:F52 A53:B53 D53:F53 A54:B54 D54:F54 A55:B55 D55:F55 A56:B56 D56:F56 A57:B57 D57:F57 A58:B58 D58:F58 A59:B59 D59:F59 A60:B60 D60:F60 A61:B61 D61:F61 A62:B62 D62:F62 A63:B63 D63:F63 A64:B64 D64:F64 A65:B65 D65:F65 A66:B66 D66:F66 A67:B67 D67:F67 A68:B68 D68:F68 A69:B69 D69:F69 A70:B70 D70:F70 A71:B71 D71:F71 A72:B72 D72:F72 A73:B73 D73:F73 A74:B74 D74:F74 A75:B75 D75:F75 A76:B76 D76:F76 A77:B77 D77:F77 A78:B78 D78:F78 A79:B79 D79:F79 A80:B80 D80:F80 A81:B81 D81:F81 A82:B82 D82:F82 A83:B83 D83:F83 A84:B84 D84:F84 A85:B85 D85:F85 A86:B86 D86:F86 A87:B87 D87:F87 A88:B88 D88:F88 A89:B89 D89:F89 A90:B90 D90:F90 A91:B91 D91:F91 A92:B92 D92:F92 A93:B93 D93:F93 A94:B94 D94:F94 A95:B95 D95:F95 A96:B96 D96:F96 D97:F97" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>